<commit_message>
Change in reporting in Hooks
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2024\Excel_6thJan\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C8F900-5CC7-4200-BF33-740D43344706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC596F74-053C-464E-896A-7E7DDFB724D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="45">
   <si>
     <t>NONSCR</t>
   </si>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,16 +608,16 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <v>360</v>
+        <v>775</v>
       </c>
       <c r="G2">
         <v>11377</v>
@@ -636,66 +636,66 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2199</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>360</v>
+      </c>
+      <c r="G3">
+        <v>11377</v>
+      </c>
+      <c r="H3">
+        <v>11377</v>
+      </c>
+      <c r="I3">
+        <v>11377</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K4">
         <v>33504984</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>775</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>360</v>
+        <v>775</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -715,22 +715,22 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2199</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>55</v>
+        <v>360</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -750,22 +750,22 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -785,95 +785,95 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
       <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <v>10763</v>
-      </c>
-      <c r="H8">
-        <v>82165</v>
-      </c>
-      <c r="I8">
-        <v>82165</v>
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
       </c>
-      <c r="K8">
-        <v>74428760</v>
-      </c>
       <c r="M8" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G9">
         <v>10763</v>
       </c>
       <c r="H9">
-        <v>10763</v>
+        <v>82165</v>
       </c>
       <c r="I9">
-        <v>10763</v>
+        <v>82165</v>
       </c>
       <c r="J9" t="s">
         <v>4</v>
       </c>
+      <c r="K9">
+        <v>74428760</v>
+      </c>
       <c r="M9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
+      <c r="D10">
+        <v>2199</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>950</v>
+        <v>120</v>
       </c>
       <c r="G10">
         <v>10763</v>
@@ -893,22 +893,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>310</v>
+        <v>950</v>
       </c>
       <c r="G11">
         <v>10763</v>
@@ -923,27 +923,27 @@
         <v>4</v>
       </c>
       <c r="M11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
       <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12">
-        <v>9730</v>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>50</v>
+        <v>310</v>
       </c>
       <c r="G12">
         <v>10763</v>
@@ -958,15 +958,15 @@
         <v>4</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -975,19 +975,19 @@
         <v>9730</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>100</v>
-      </c>
-      <c r="G13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>10763</v>
+      </c>
+      <c r="H13">
+        <v>10763</v>
+      </c>
+      <c r="I13">
+        <v>10763</v>
       </c>
       <c r="J13" t="s">
         <v>4</v>
@@ -998,10 +998,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1013,13 +1013,13 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>35</v>
-      </c>
-      <c r="G14">
-        <v>49990</v>
-      </c>
-      <c r="H14">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
       </c>
       <c r="I14" t="s">
         <v>6</v>
@@ -1033,40 +1033,37 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>9730</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G15">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H15">
-        <v>10763</v>
-      </c>
-      <c r="I15">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
       </c>
       <c r="J15" t="s">
         <v>4</v>
       </c>
-      <c r="L15" t="s">
-        <v>5</v>
-      </c>
       <c r="M15" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -1074,19 +1071,19 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="D16">
-        <v>2199</v>
+      <c r="D16" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>360</v>
+        <v>20</v>
       </c>
       <c r="G16">
         <v>10763</v>
@@ -1100,28 +1097,31 @@
       <c r="J16" t="s">
         <v>4</v>
       </c>
+      <c r="L16" t="s">
+        <v>5</v>
+      </c>
       <c r="M16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>2199</v>
       </c>
       <c r="E17">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G17">
         <v>10763</v>
@@ -1141,22 +1141,22 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F18">
-        <v>56</v>
+        <v>775</v>
       </c>
       <c r="G18">
         <v>10763</v>
@@ -1176,22 +1176,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>180</v>
+        <v>56</v>
       </c>
       <c r="G19">
         <v>10763</v>
@@ -1214,33 +1214,68 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>180</v>
+      </c>
+      <c r="G20">
+        <v>10763</v>
+      </c>
+      <c r="H20">
+        <v>10763</v>
+      </c>
+      <c r="I20">
+        <v>10763</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>31</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>4340</v>
       </c>
-      <c r="G20">
-        <v>10763</v>
-      </c>
-      <c r="H20">
-        <v>10763</v>
-      </c>
-      <c r="I20">
-        <v>10763</v>
-      </c>
-      <c r="J20" t="s">
-        <v>4</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="G21">
+        <v>10763</v>
+      </c>
+      <c r="H21">
+        <v>10763</v>
+      </c>
+      <c r="I21">
+        <v>10763</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented data reading config from blobs
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2024\Excel_6thJan\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC596F74-053C-464E-896A-7E7DDFB724D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3360999D-E97A-4AC3-A132-3D342547EC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="45">
   <si>
     <t>NONSCR</t>
   </si>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,22 +637,22 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>2199</v>
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F3">
-        <v>360</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>11377</v>
@@ -671,66 +671,66 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2199</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>360</v>
+      </c>
+      <c r="G4">
+        <v>11377</v>
+      </c>
+      <c r="H4">
+        <v>11377</v>
+      </c>
+      <c r="I4">
+        <v>11377</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K5">
         <v>33504984</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M5" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>775</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>360</v>
+        <v>775</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -750,22 +750,22 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2199</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>55</v>
+        <v>360</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -785,22 +785,22 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -820,95 +820,95 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>10763</v>
-      </c>
-      <c r="H9">
-        <v>82165</v>
-      </c>
-      <c r="I9">
-        <v>82165</v>
+        <v>90</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>4</v>
       </c>
-      <c r="K9">
-        <v>74428760</v>
-      </c>
       <c r="M9" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G10">
         <v>10763</v>
       </c>
       <c r="H10">
-        <v>10763</v>
+        <v>82165</v>
       </c>
       <c r="I10">
-        <v>10763</v>
+        <v>82165</v>
       </c>
       <c r="J10" t="s">
         <v>4</v>
       </c>
+      <c r="K10">
+        <v>74428760</v>
+      </c>
       <c r="M10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
+      <c r="D11">
+        <v>2199</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>950</v>
+        <v>120</v>
       </c>
       <c r="G11">
         <v>10763</v>
@@ -928,22 +928,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F12">
-        <v>310</v>
+        <v>950</v>
       </c>
       <c r="G12">
         <v>10763</v>
@@ -958,27 +958,27 @@
         <v>4</v>
       </c>
       <c r="M12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13">
-        <v>9730</v>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>50</v>
+        <v>310</v>
       </c>
       <c r="G13">
         <v>10763</v>
@@ -993,15 +993,15 @@
         <v>4</v>
       </c>
       <c r="M13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1010,19 +1010,19 @@
         <v>9730</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>100</v>
-      </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>10763</v>
+      </c>
+      <c r="H14">
+        <v>10763</v>
+      </c>
+      <c r="I14">
+        <v>10763</v>
       </c>
       <c r="J14" t="s">
         <v>4</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -1048,13 +1048,13 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>35</v>
-      </c>
-      <c r="G15">
-        <v>49990</v>
-      </c>
-      <c r="H15">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
       </c>
       <c r="I15" t="s">
         <v>6</v>
@@ -1068,40 +1068,37 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>9730</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G16">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H16">
-        <v>10763</v>
-      </c>
-      <c r="I16">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
       </c>
       <c r="J16" t="s">
         <v>4</v>
       </c>
-      <c r="L16" t="s">
-        <v>5</v>
-      </c>
       <c r="M16" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
@@ -1109,19 +1106,19 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17">
-        <v>2199</v>
+      <c r="D17" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>360</v>
+        <v>20</v>
       </c>
       <c r="G17">
         <v>10763</v>
@@ -1135,28 +1132,31 @@
       <c r="J17" t="s">
         <v>4</v>
       </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
       <c r="M17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2199</v>
       </c>
       <c r="E18">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G18">
         <v>10763</v>
@@ -1176,22 +1176,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F19">
-        <v>56</v>
+        <v>775</v>
       </c>
       <c r="G19">
         <v>10763</v>
@@ -1211,22 +1211,22 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>180</v>
+        <v>56</v>
       </c>
       <c r="G20">
         <v>10763</v>
@@ -1249,33 +1249,68 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>180</v>
+      </c>
+      <c r="G21">
+        <v>10763</v>
+      </c>
+      <c r="H21">
+        <v>10763</v>
+      </c>
+      <c r="I21">
+        <v>10763</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>31</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>4340</v>
       </c>
-      <c r="G21">
-        <v>10763</v>
-      </c>
-      <c r="H21">
-        <v>10763</v>
-      </c>
-      <c r="I21">
-        <v>10763</v>
-      </c>
-      <c r="J21" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="G22">
+        <v>10763</v>
+      </c>
+      <c r="H22">
+        <v>10763</v>
+      </c>
+      <c r="I22">
+        <v>10763</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change in opr344 feature
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2024\Excel_6thJan\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8104FC6-ACD0-4E65-AC67-B5AB6B8DD921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924A2545-D29A-4E52-8C8F-5E25AD573DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
   <sheets>
     <sheet name="CAP018_BKG_00001" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CAP018_BKG_00001!$A$1:$M$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CAP018_BKG_00001!$A$1:$M$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="45">
   <si>
     <t>NONSCR</t>
   </si>
@@ -547,11 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2076,22 +2075,22 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F44">
-        <v>360</v>
+        <v>12</v>
       </c>
       <c r="G44">
         <v>11377</v>
@@ -2117,16 +2116,16 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F45">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G45">
         <v>11377</v>
@@ -2146,13 +2145,13 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D46" t="s">
         <v>0</v>
@@ -2161,7 +2160,7 @@
         <v>13</v>
       </c>
       <c r="F46">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G46">
         <v>11377</v>
@@ -2184,19 +2183,19 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F47">
-        <v>360</v>
+        <v>12</v>
       </c>
       <c r="G47">
         <v>11377</v>
@@ -2216,22 +2215,22 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D48" t="s">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F48">
-        <v>10</v>
+        <v>360</v>
       </c>
       <c r="G48">
         <v>11377</v>
@@ -2251,13 +2250,13 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49" t="s">
         <v>0</v>
@@ -2266,7 +2265,7 @@
         <v>13</v>
       </c>
       <c r="F49">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G49">
         <v>11377</v>
@@ -2289,19 +2288,19 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F50">
-        <v>360</v>
+        <v>12</v>
       </c>
       <c r="G50">
         <v>11377</v>
@@ -2327,16 +2326,16 @@
         <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D51" t="s">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>360</v>
       </c>
       <c r="G51">
         <v>11377</v>
@@ -2359,7 +2358,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -2371,7 +2370,7 @@
         <v>13</v>
       </c>
       <c r="F52">
-        <v>12</v>
+        <v>775</v>
       </c>
       <c r="G52">
         <v>11377</v>
@@ -2391,10 +2390,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -2403,44 +2402,71 @@
         <v>0</v>
       </c>
       <c r="E53">
+        <v>13</v>
+      </c>
+      <c r="F53">
+        <v>100</v>
+      </c>
+      <c r="G53">
+        <v>11377</v>
+      </c>
+      <c r="H53">
+        <v>11377</v>
+      </c>
+      <c r="I53">
+        <v>11377</v>
+      </c>
+      <c r="J53" t="s">
+        <v>4</v>
+      </c>
+      <c r="M53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>2199</v>
+      </c>
+      <c r="E54">
         <v>10</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>360</v>
       </c>
-      <c r="G53">
-        <v>11377</v>
-      </c>
-      <c r="H53">
-        <v>11377</v>
-      </c>
-      <c r="I53">
-        <v>11377</v>
-      </c>
-      <c r="J53" t="s">
-        <v>4</v>
-      </c>
-      <c r="M53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="K54">
-        <v>33504984</v>
+      <c r="G54">
+        <v>11377</v>
+      </c>
+      <c r="H54">
+        <v>11377</v>
+      </c>
+      <c r="I54">
+        <v>11377</v>
+      </c>
+      <c r="J54" t="s">
+        <v>4</v>
       </c>
       <c r="M54" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
         <v>0</v>
@@ -2449,22 +2475,22 @@
         <v>13</v>
       </c>
       <c r="F55">
-        <v>775</v>
-      </c>
-      <c r="G55" t="s">
-        <v>5</v>
-      </c>
-      <c r="H55" t="s">
-        <v>6</v>
-      </c>
-      <c r="I55" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="G55">
+        <v>11377</v>
+      </c>
+      <c r="H55">
+        <v>11377</v>
+      </c>
+      <c r="I55">
+        <v>11377</v>
       </c>
       <c r="J55" t="s">
         <v>4</v>
       </c>
       <c r="M55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
@@ -2475,39 +2501,39 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56">
-        <v>2199</v>
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F56">
-        <v>360</v>
-      </c>
-      <c r="G56" t="s">
-        <v>5</v>
-      </c>
-      <c r="H56" t="s">
-        <v>6</v>
-      </c>
-      <c r="I56" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="G56">
+        <v>11377</v>
+      </c>
+      <c r="H56">
+        <v>11377</v>
+      </c>
+      <c r="I56">
+        <v>11377</v>
       </c>
       <c r="J56" t="s">
         <v>4</v>
       </c>
       <c r="M56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
         <v>26</v>
@@ -2516,30 +2542,30 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F57">
-        <v>55</v>
-      </c>
-      <c r="G57" t="s">
-        <v>5</v>
-      </c>
-      <c r="H57" t="s">
-        <v>6</v>
-      </c>
-      <c r="I57" t="s">
-        <v>6</v>
+        <v>360</v>
+      </c>
+      <c r="G57">
+        <v>11377</v>
+      </c>
+      <c r="H57">
+        <v>11377</v>
+      </c>
+      <c r="I57">
+        <v>11377</v>
       </c>
       <c r="J57" t="s">
         <v>4</v>
       </c>
       <c r="M57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
         <v>23</v>
@@ -2551,25 +2577,25 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F58">
-        <v>90</v>
-      </c>
-      <c r="G58" t="s">
-        <v>5</v>
-      </c>
-      <c r="H58" t="s">
-        <v>6</v>
-      </c>
-      <c r="I58" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="G58">
+        <v>11377</v>
+      </c>
+      <c r="H58">
+        <v>11377</v>
+      </c>
+      <c r="I58">
+        <v>11377</v>
       </c>
       <c r="J58" t="s">
         <v>4</v>
       </c>
       <c r="M58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
@@ -2577,7 +2603,7 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -2589,112 +2615,85 @@
         <v>13</v>
       </c>
       <c r="F59">
-        <v>775</v>
-      </c>
-      <c r="G59" t="s">
-        <v>5</v>
-      </c>
-      <c r="H59" t="s">
-        <v>6</v>
-      </c>
-      <c r="I59" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="G59">
+        <v>11377</v>
+      </c>
+      <c r="H59">
+        <v>11377</v>
+      </c>
+      <c r="I59">
+        <v>11377</v>
       </c>
       <c r="J59" t="s">
         <v>4</v>
       </c>
       <c r="M59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60">
-        <v>2199</v>
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F60">
         <v>360</v>
       </c>
-      <c r="G60" t="s">
-        <v>5</v>
-      </c>
-      <c r="H60" t="s">
-        <v>6</v>
-      </c>
-      <c r="I60" t="s">
-        <v>6</v>
+      <c r="G60">
+        <v>11377</v>
+      </c>
+      <c r="H60">
+        <v>11377</v>
+      </c>
+      <c r="I60">
+        <v>11377</v>
       </c>
       <c r="J60" t="s">
         <v>4</v>
       </c>
       <c r="M60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>24</v>
-      </c>
-      <c r="B61" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" t="s">
-        <v>26</v>
-      </c>
-      <c r="D61" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
-      <c r="F61">
-        <v>55</v>
-      </c>
-      <c r="G61" t="s">
-        <v>5</v>
-      </c>
-      <c r="H61" t="s">
-        <v>6</v>
-      </c>
-      <c r="I61" t="s">
-        <v>6</v>
-      </c>
-      <c r="J61" t="s">
-        <v>4</v>
+      <c r="K61">
+        <v>33504984</v>
       </c>
       <c r="M61" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F62">
-        <v>90</v>
+        <v>775</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
@@ -2714,22 +2713,22 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>2199</v>
       </c>
       <c r="E63">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F63">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
@@ -2749,22 +2748,22 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64">
-        <v>2199</v>
+        <v>26</v>
+      </c>
+      <c r="D64" t="s">
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F64">
-        <v>360</v>
+        <v>55</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
@@ -2784,22 +2783,22 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D65" t="s">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
@@ -2819,22 +2818,22 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D66" t="s">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F66">
-        <v>90</v>
+        <v>775</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
@@ -2854,22 +2853,22 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>2199</v>
       </c>
       <c r="E67">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F67">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
@@ -2889,22 +2888,22 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C68" t="s">
-        <v>3</v>
-      </c>
-      <c r="D68">
-        <v>2199</v>
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F68">
-        <v>360</v>
+        <v>55</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
@@ -2924,22 +2923,22 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F69">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
@@ -2959,22 +2958,22 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F70">
-        <v>90</v>
+        <v>775</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
@@ -2994,22 +2993,22 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>2199</v>
       </c>
       <c r="E71">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F71">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
@@ -3029,22 +3028,22 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72">
-        <v>2199</v>
+        <v>26</v>
+      </c>
+      <c r="D72" t="s">
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F72">
-        <v>360</v>
+        <v>55</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
@@ -3064,22 +3063,22 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C73" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D73" t="s">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F73">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
@@ -3099,22 +3098,22 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D74" t="s">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F74">
-        <v>90</v>
+        <v>775</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
@@ -3134,22 +3133,22 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>2199</v>
       </c>
       <c r="E75">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F75">
-        <v>775</v>
+        <v>360</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
@@ -3169,22 +3168,22 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76">
-        <v>2199</v>
+        <v>26</v>
+      </c>
+      <c r="D76" t="s">
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F76">
-        <v>360</v>
+        <v>55</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
@@ -3204,22 +3203,22 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B77" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D77" t="s">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F77">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
@@ -3239,22 +3238,22 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F78">
-        <v>90</v>
+        <v>775</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
@@ -3272,147 +3271,144 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>23</v>
       </c>
       <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79">
+        <v>2199</v>
+      </c>
+      <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="F79">
+        <v>360</v>
+      </c>
+      <c r="G79" t="s">
+        <v>5</v>
+      </c>
+      <c r="H79" t="s">
+        <v>6</v>
+      </c>
+      <c r="I79" t="s">
+        <v>6</v>
+      </c>
+      <c r="J79" t="s">
+        <v>4</v>
+      </c>
+      <c r="M79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80">
+        <v>55</v>
+      </c>
+      <c r="G80" t="s">
+        <v>5</v>
+      </c>
+      <c r="H80" t="s">
+        <v>6</v>
+      </c>
+      <c r="I80" t="s">
+        <v>6</v>
+      </c>
+      <c r="J80" t="s">
+        <v>4</v>
+      </c>
+      <c r="M80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>27</v>
       </c>
-      <c r="C79" t="s">
-        <v>1</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E79">
-        <v>2</v>
-      </c>
-      <c r="F79">
-        <v>20</v>
-      </c>
-      <c r="G79">
-        <v>10763</v>
-      </c>
-      <c r="H79">
-        <v>82165</v>
-      </c>
-      <c r="I79">
-        <v>82165</v>
-      </c>
-      <c r="J79" t="s">
-        <v>4</v>
-      </c>
-      <c r="K79">
-        <v>74428760</v>
-      </c>
-      <c r="M79" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" t="s">
-        <v>34</v>
-      </c>
-      <c r="C80" t="s">
-        <v>3</v>
-      </c>
-      <c r="D80">
-        <v>2199</v>
-      </c>
-      <c r="E80">
-        <v>4</v>
-      </c>
-      <c r="F80">
-        <v>120</v>
-      </c>
-      <c r="G80">
-        <v>10763</v>
-      </c>
-      <c r="H80">
-        <v>10763</v>
-      </c>
-      <c r="I80">
-        <v>10763</v>
-      </c>
-      <c r="J80" t="s">
-        <v>4</v>
-      </c>
-      <c r="M80" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>36</v>
-      </c>
       <c r="B81" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C81" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>43</v>
+      <c r="D81" t="s">
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F81">
-        <v>950</v>
-      </c>
-      <c r="G81">
-        <v>10763</v>
-      </c>
-      <c r="H81">
-        <v>10763</v>
-      </c>
-      <c r="I81">
-        <v>10763</v>
+        <v>90</v>
+      </c>
+      <c r="G81" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" t="s">
+        <v>6</v>
       </c>
       <c r="J81" t="s">
         <v>4</v>
       </c>
       <c r="M81" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>44</v>
+      <c r="D82" t="s">
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F82">
-        <v>310</v>
-      </c>
-      <c r="G82">
-        <v>10763</v>
-      </c>
-      <c r="H82">
-        <v>10763</v>
-      </c>
-      <c r="I82">
-        <v>10763</v>
+        <v>775</v>
+      </c>
+      <c r="G82" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" t="s">
+        <v>6</v>
+      </c>
+      <c r="I82" t="s">
+        <v>6</v>
       </c>
       <c r="J82" t="s">
         <v>4</v>
       </c>
       <c r="M82" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
@@ -3420,54 +3416,54 @@
         <v>23</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D83">
-        <v>9730</v>
+        <v>2199</v>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F83">
-        <v>50</v>
-      </c>
-      <c r="G83">
-        <v>10763</v>
-      </c>
-      <c r="H83">
-        <v>10763</v>
-      </c>
-      <c r="I83">
-        <v>10763</v>
+        <v>360</v>
+      </c>
+      <c r="G83" t="s">
+        <v>5</v>
+      </c>
+      <c r="H83" t="s">
+        <v>6</v>
+      </c>
+      <c r="I83" t="s">
+        <v>6</v>
       </c>
       <c r="J83" t="s">
         <v>4</v>
       </c>
       <c r="M83" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B84" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
-      </c>
-      <c r="D84">
-        <v>9730</v>
+        <v>26</v>
+      </c>
+      <c r="D84" t="s">
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F84">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
@@ -3482,33 +3478,33 @@
         <v>4</v>
       </c>
       <c r="M84" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
-      </c>
-      <c r="D85">
-        <v>9730</v>
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F85">
-        <v>35</v>
-      </c>
-      <c r="G85">
-        <v>49990</v>
-      </c>
-      <c r="H85">
-        <v>49990</v>
+        <v>90</v>
+      </c>
+      <c r="G85" t="s">
+        <v>5</v>
+      </c>
+      <c r="H85" t="s">
+        <v>6</v>
       </c>
       <c r="I85" t="s">
         <v>6</v>
@@ -3517,7 +3513,7 @@
         <v>4</v>
       </c>
       <c r="M85" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
@@ -3528,31 +3524,34 @@
         <v>27</v>
       </c>
       <c r="C86" t="s">
-        <v>28</v>
-      </c>
-      <c r="D86">
-        <v>9730</v>
+        <v>1</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E86">
         <v>2</v>
       </c>
       <c r="F86">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G86">
         <v>10763</v>
       </c>
       <c r="H86">
-        <v>10763</v>
+        <v>82165</v>
       </c>
       <c r="I86">
-        <v>10763</v>
+        <v>82165</v>
       </c>
       <c r="J86" t="s">
         <v>4</v>
       </c>
+      <c r="K86">
+        <v>74428760</v>
+      </c>
       <c r="M86" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
@@ -3560,89 +3559,89 @@
         <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C87" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D87">
-        <v>9730</v>
+        <v>2199</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F87">
-        <v>100</v>
-      </c>
-      <c r="G87" t="s">
-        <v>5</v>
-      </c>
-      <c r="H87" t="s">
-        <v>6</v>
-      </c>
-      <c r="I87" t="s">
-        <v>6</v>
+        <v>120</v>
+      </c>
+      <c r="G87">
+        <v>10763</v>
+      </c>
+      <c r="H87">
+        <v>10763</v>
+      </c>
+      <c r="I87">
+        <v>10763</v>
       </c>
       <c r="J87" t="s">
         <v>4</v>
       </c>
       <c r="M87" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
-      </c>
-      <c r="D88">
-        <v>9730</v>
+        <v>3</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F88">
+        <v>950</v>
+      </c>
+      <c r="G88">
+        <v>10763</v>
+      </c>
+      <c r="H88">
+        <v>10763</v>
+      </c>
+      <c r="I88">
+        <v>10763</v>
+      </c>
+      <c r="J88" t="s">
+        <v>4</v>
+      </c>
+      <c r="M88" t="s">
         <v>35</v>
-      </c>
-      <c r="G88">
-        <v>49990</v>
-      </c>
-      <c r="H88">
-        <v>49990</v>
-      </c>
-      <c r="I88" t="s">
-        <v>6</v>
-      </c>
-      <c r="J88" t="s">
-        <v>4</v>
-      </c>
-      <c r="M88" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B89" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
-      </c>
-      <c r="D89">
-        <v>9730</v>
+        <v>1</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E89">
         <v>2</v>
       </c>
       <c r="F89">
-        <v>50</v>
+        <v>310</v>
       </c>
       <c r="G89">
         <v>10763</v>
@@ -3657,15 +3656,15 @@
         <v>4</v>
       </c>
       <c r="M89" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B90" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -3674,19 +3673,19 @@
         <v>9730</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F90">
-        <v>100</v>
-      </c>
-      <c r="G90" t="s">
-        <v>5</v>
-      </c>
-      <c r="H90" t="s">
-        <v>6</v>
-      </c>
-      <c r="I90" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G90">
+        <v>10763</v>
+      </c>
+      <c r="H90">
+        <v>10763</v>
+      </c>
+      <c r="I90">
+        <v>10763</v>
       </c>
       <c r="J90" t="s">
         <v>4</v>
@@ -3697,10 +3696,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
@@ -3712,13 +3711,13 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>35</v>
-      </c>
-      <c r="G91">
-        <v>49990</v>
-      </c>
-      <c r="H91">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G91" t="s">
+        <v>5</v>
+      </c>
+      <c r="H91" t="s">
+        <v>6</v>
       </c>
       <c r="I91" t="s">
         <v>6</v>
@@ -3732,10 +3731,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B92" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C92" t="s">
         <v>28</v>
@@ -3744,19 +3743,19 @@
         <v>9730</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G92">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H92">
-        <v>10763</v>
-      </c>
-      <c r="I92">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I92" t="s">
+        <v>6</v>
       </c>
       <c r="J92" t="s">
         <v>4</v>
@@ -3767,10 +3766,10 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B93" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C93" t="s">
         <v>28</v>
@@ -3779,19 +3778,19 @@
         <v>9730</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F93">
-        <v>100</v>
-      </c>
-      <c r="G93" t="s">
-        <v>5</v>
-      </c>
-      <c r="H93" t="s">
-        <v>6</v>
-      </c>
-      <c r="I93" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G93">
+        <v>10763</v>
+      </c>
+      <c r="H93">
+        <v>10763</v>
+      </c>
+      <c r="I93">
+        <v>10763</v>
       </c>
       <c r="J93" t="s">
         <v>4</v>
@@ -3802,10 +3801,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C94" t="s">
         <v>28</v>
@@ -3817,13 +3816,13 @@
         <v>1</v>
       </c>
       <c r="F94">
-        <v>35</v>
-      </c>
-      <c r="G94">
-        <v>49990</v>
-      </c>
-      <c r="H94">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G94" t="s">
+        <v>5</v>
+      </c>
+      <c r="H94" t="s">
+        <v>6</v>
       </c>
       <c r="I94" t="s">
         <v>6</v>
@@ -3837,10 +3836,10 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C95" t="s">
         <v>28</v>
@@ -3849,19 +3848,19 @@
         <v>9730</v>
       </c>
       <c r="E95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G95">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H95">
-        <v>10763</v>
-      </c>
-      <c r="I95">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I95" t="s">
+        <v>6</v>
       </c>
       <c r="J95" t="s">
         <v>4</v>
@@ -3872,10 +3871,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C96" t="s">
         <v>28</v>
@@ -3884,19 +3883,19 @@
         <v>9730</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F96">
-        <v>100</v>
-      </c>
-      <c r="G96" t="s">
-        <v>5</v>
-      </c>
-      <c r="H96" t="s">
-        <v>6</v>
-      </c>
-      <c r="I96" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G96">
+        <v>10763</v>
+      </c>
+      <c r="H96">
+        <v>10763</v>
+      </c>
+      <c r="I96">
+        <v>10763</v>
       </c>
       <c r="J96" t="s">
         <v>4</v>
@@ -3907,10 +3906,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -3922,13 +3921,13 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>35</v>
-      </c>
-      <c r="G97">
-        <v>49990</v>
-      </c>
-      <c r="H97">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G97" t="s">
+        <v>5</v>
+      </c>
+      <c r="H97" t="s">
+        <v>6</v>
       </c>
       <c r="I97" t="s">
         <v>6</v>
@@ -3942,10 +3941,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -3954,19 +3953,19 @@
         <v>9730</v>
       </c>
       <c r="E98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G98">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H98">
-        <v>10763</v>
-      </c>
-      <c r="I98">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I98" t="s">
+        <v>6</v>
       </c>
       <c r="J98" t="s">
         <v>4</v>
@@ -3977,10 +3976,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -3989,19 +3988,19 @@
         <v>9730</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F99">
-        <v>100</v>
-      </c>
-      <c r="G99" t="s">
-        <v>5</v>
-      </c>
-      <c r="H99" t="s">
-        <v>6</v>
-      </c>
-      <c r="I99" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G99">
+        <v>10763</v>
+      </c>
+      <c r="H99">
+        <v>10763</v>
+      </c>
+      <c r="I99">
+        <v>10763</v>
       </c>
       <c r="J99" t="s">
         <v>4</v>
@@ -4012,10 +4011,10 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -4027,13 +4026,13 @@
         <v>1</v>
       </c>
       <c r="F100">
-        <v>35</v>
-      </c>
-      <c r="G100">
-        <v>49990</v>
-      </c>
-      <c r="H100">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G100" t="s">
+        <v>5</v>
+      </c>
+      <c r="H100" t="s">
+        <v>6</v>
       </c>
       <c r="I100" t="s">
         <v>6</v>
@@ -4047,10 +4046,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C101" t="s">
         <v>28</v>
@@ -4059,19 +4058,19 @@
         <v>9730</v>
       </c>
       <c r="E101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F101">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G101">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H101">
-        <v>10763</v>
-      </c>
-      <c r="I101">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I101" t="s">
+        <v>6</v>
       </c>
       <c r="J101" t="s">
         <v>4</v>
@@ -4082,10 +4081,10 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B102" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C102" t="s">
         <v>28</v>
@@ -4094,19 +4093,19 @@
         <v>9730</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F102">
-        <v>100</v>
-      </c>
-      <c r="G102" t="s">
-        <v>5</v>
-      </c>
-      <c r="H102" t="s">
-        <v>6</v>
-      </c>
-      <c r="I102" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G102">
+        <v>10763</v>
+      </c>
+      <c r="H102">
+        <v>10763</v>
+      </c>
+      <c r="I102">
+        <v>10763</v>
       </c>
       <c r="J102" t="s">
         <v>4</v>
@@ -4117,10 +4116,10 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C103" t="s">
         <v>28</v>
@@ -4132,13 +4131,13 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>35</v>
-      </c>
-      <c r="G103">
-        <v>49990</v>
-      </c>
-      <c r="H103">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G103" t="s">
+        <v>5</v>
+      </c>
+      <c r="H103" t="s">
+        <v>6</v>
       </c>
       <c r="I103" t="s">
         <v>6</v>
@@ -4152,10 +4151,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B104" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -4164,19 +4163,19 @@
         <v>9730</v>
       </c>
       <c r="E104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F104">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G104">
-        <v>10763</v>
+        <v>49990</v>
       </c>
       <c r="H104">
-        <v>10763</v>
-      </c>
-      <c r="I104">
-        <v>10763</v>
+        <v>49990</v>
+      </c>
+      <c r="I104" t="s">
+        <v>6</v>
       </c>
       <c r="J104" t="s">
         <v>4</v>
@@ -4187,10 +4186,10 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B105" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -4199,19 +4198,19 @@
         <v>9730</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F105">
-        <v>100</v>
-      </c>
-      <c r="G105" t="s">
-        <v>5</v>
-      </c>
-      <c r="H105" t="s">
-        <v>6</v>
-      </c>
-      <c r="I105" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="G105">
+        <v>10763</v>
+      </c>
+      <c r="H105">
+        <v>10763</v>
+      </c>
+      <c r="I105">
+        <v>10763</v>
       </c>
       <c r="J105" t="s">
         <v>4</v>
@@ -4222,10 +4221,10 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
@@ -4237,13 +4236,13 @@
         <v>1</v>
       </c>
       <c r="F106">
-        <v>35</v>
-      </c>
-      <c r="G106">
-        <v>49990</v>
-      </c>
-      <c r="H106">
-        <v>49990</v>
+        <v>100</v>
+      </c>
+      <c r="G106" t="s">
+        <v>5</v>
+      </c>
+      <c r="H106" t="s">
+        <v>6</v>
       </c>
       <c r="I106" t="s">
         <v>6</v>
@@ -4255,229 +4254,675 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B107" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C107" t="s">
+        <v>28</v>
+      </c>
+      <c r="D107">
+        <v>9730</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>35</v>
+      </c>
+      <c r="G107">
+        <v>49990</v>
+      </c>
+      <c r="H107">
+        <v>49990</v>
+      </c>
+      <c r="I107" t="s">
+        <v>6</v>
+      </c>
+      <c r="J107" t="s">
+        <v>4</v>
+      </c>
+      <c r="M107" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" t="s">
+        <v>27</v>
+      </c>
+      <c r="C108" t="s">
+        <v>28</v>
+      </c>
+      <c r="D108">
+        <v>9730</v>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+      <c r="F108">
+        <v>50</v>
+      </c>
+      <c r="G108">
+        <v>10763</v>
+      </c>
+      <c r="H108">
+        <v>10763</v>
+      </c>
+      <c r="I108">
+        <v>10763</v>
+      </c>
+      <c r="J108" t="s">
+        <v>4</v>
+      </c>
+      <c r="M108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" t="s">
+        <v>28</v>
+      </c>
+      <c r="D109">
+        <v>9730</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>100</v>
+      </c>
+      <c r="G109" t="s">
+        <v>5</v>
+      </c>
+      <c r="H109" t="s">
+        <v>6</v>
+      </c>
+      <c r="I109" t="s">
+        <v>6</v>
+      </c>
+      <c r="J109" t="s">
+        <v>4</v>
+      </c>
+      <c r="M109" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>28</v>
+      </c>
+      <c r="D110">
+        <v>9730</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>35</v>
+      </c>
+      <c r="G110">
+        <v>49990</v>
+      </c>
+      <c r="H110">
+        <v>49990</v>
+      </c>
+      <c r="I110" t="s">
+        <v>6</v>
+      </c>
+      <c r="J110" t="s">
+        <v>4</v>
+      </c>
+      <c r="M110" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>27</v>
+      </c>
+      <c r="C111" t="s">
+        <v>28</v>
+      </c>
+      <c r="D111">
+        <v>9730</v>
+      </c>
+      <c r="E111">
+        <v>2</v>
+      </c>
+      <c r="F111">
+        <v>50</v>
+      </c>
+      <c r="G111">
+        <v>10763</v>
+      </c>
+      <c r="H111">
+        <v>10763</v>
+      </c>
+      <c r="I111">
+        <v>10763</v>
+      </c>
+      <c r="J111" t="s">
+        <v>4</v>
+      </c>
+      <c r="M111" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" t="s">
+        <v>30</v>
+      </c>
+      <c r="C112" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112">
+        <v>9730</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>100</v>
+      </c>
+      <c r="G112" t="s">
+        <v>5</v>
+      </c>
+      <c r="H112" t="s">
+        <v>6</v>
+      </c>
+      <c r="I112" t="s">
+        <v>6</v>
+      </c>
+      <c r="J112" t="s">
+        <v>4</v>
+      </c>
+      <c r="M112" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>31</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>28</v>
+      </c>
+      <c r="D113">
+        <v>9730</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>35</v>
+      </c>
+      <c r="G113">
+        <v>49990</v>
+      </c>
+      <c r="H113">
+        <v>49990</v>
+      </c>
+      <c r="I113" t="s">
+        <v>6</v>
+      </c>
+      <c r="J113" t="s">
+        <v>4</v>
+      </c>
+      <c r="M113" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" t="s">
+        <v>28</v>
+      </c>
+      <c r="D114">
+        <v>9730</v>
+      </c>
+      <c r="E114">
+        <v>2</v>
+      </c>
+      <c r="F114">
+        <v>50</v>
+      </c>
+      <c r="G114">
+        <v>10763</v>
+      </c>
+      <c r="H114">
+        <v>10763</v>
+      </c>
+      <c r="I114">
+        <v>10763</v>
+      </c>
+      <c r="J114" t="s">
+        <v>4</v>
+      </c>
+      <c r="M114" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" t="s">
+        <v>30</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115">
+        <v>9730</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>100</v>
+      </c>
+      <c r="G115" t="s">
+        <v>5</v>
+      </c>
+      <c r="H115" t="s">
+        <v>6</v>
+      </c>
+      <c r="I115" t="s">
+        <v>6</v>
+      </c>
+      <c r="J115" t="s">
+        <v>4</v>
+      </c>
+      <c r="M115" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>31</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>28</v>
+      </c>
+      <c r="D116">
+        <v>9730</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>35</v>
+      </c>
+      <c r="G116">
+        <v>49990</v>
+      </c>
+      <c r="H116">
+        <v>49990</v>
+      </c>
+      <c r="I116" t="s">
+        <v>6</v>
+      </c>
+      <c r="J116" t="s">
+        <v>4</v>
+      </c>
+      <c r="M116" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>27</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117">
+        <v>9730</v>
+      </c>
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="F117">
+        <v>50</v>
+      </c>
+      <c r="G117">
+        <v>10763</v>
+      </c>
+      <c r="H117">
+        <v>10763</v>
+      </c>
+      <c r="I117">
+        <v>10763</v>
+      </c>
+      <c r="J117" t="s">
+        <v>4</v>
+      </c>
+      <c r="M117" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" t="s">
+        <v>30</v>
+      </c>
+      <c r="C118" t="s">
+        <v>28</v>
+      </c>
+      <c r="D118">
+        <v>9730</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>100</v>
+      </c>
+      <c r="G118" t="s">
+        <v>5</v>
+      </c>
+      <c r="H118" t="s">
+        <v>6</v>
+      </c>
+      <c r="I118" t="s">
+        <v>6</v>
+      </c>
+      <c r="J118" t="s">
+        <v>4</v>
+      </c>
+      <c r="M118" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>31</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119">
+        <v>9730</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>35</v>
+      </c>
+      <c r="G119">
+        <v>49990</v>
+      </c>
+      <c r="H119">
+        <v>49990</v>
+      </c>
+      <c r="I119" t="s">
+        <v>6</v>
+      </c>
+      <c r="J119" t="s">
+        <v>4</v>
+      </c>
+      <c r="M119" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E107">
-        <v>2</v>
-      </c>
-      <c r="F107">
+      <c r="E120">
+        <v>2</v>
+      </c>
+      <c r="F120">
         <v>20</v>
       </c>
-      <c r="G107">
-        <v>10763</v>
-      </c>
-      <c r="H107">
-        <v>10763</v>
-      </c>
-      <c r="I107">
-        <v>10763</v>
-      </c>
-      <c r="J107" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" t="s">
+      <c r="G120">
+        <v>10763</v>
+      </c>
+      <c r="H120">
+        <v>10763</v>
+      </c>
+      <c r="I120">
+        <v>10763</v>
+      </c>
+      <c r="J120" t="s">
+        <v>4</v>
+      </c>
+      <c r="L120" t="s">
         <v>5</v>
       </c>
-      <c r="M107" t="s">
+      <c r="M120" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
-        <v>23</v>
-      </c>
-      <c r="B108" t="s">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" t="s">
         <v>30</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C121" t="s">
         <v>3</v>
       </c>
-      <c r="D108">
+      <c r="D121">
         <v>2199</v>
       </c>
-      <c r="E108">
+      <c r="E121">
         <v>10</v>
       </c>
-      <c r="F108">
+      <c r="F121">
         <v>360</v>
       </c>
-      <c r="G108">
-        <v>10763</v>
-      </c>
-      <c r="H108">
-        <v>10763</v>
-      </c>
-      <c r="I108">
-        <v>10763</v>
-      </c>
-      <c r="J108" t="s">
-        <v>4</v>
-      </c>
-      <c r="M108" t="s">
+      <c r="G121">
+        <v>10763</v>
+      </c>
+      <c r="H121">
+        <v>10763</v>
+      </c>
+      <c r="I121">
+        <v>10763</v>
+      </c>
+      <c r="J121" t="s">
+        <v>4</v>
+      </c>
+      <c r="M121" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" t="s">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" t="s">
         <v>31</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C122" t="s">
         <v>1</v>
       </c>
-      <c r="D109" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109">
+      <c r="D122" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122">
         <v>13</v>
       </c>
-      <c r="F109">
+      <c r="F122">
         <v>775</v>
       </c>
-      <c r="G109">
-        <v>10763</v>
-      </c>
-      <c r="H109">
-        <v>10763</v>
-      </c>
-      <c r="I109">
-        <v>10763</v>
-      </c>
-      <c r="J109" t="s">
-        <v>4</v>
-      </c>
-      <c r="M109" t="s">
+      <c r="G122">
+        <v>10763</v>
+      </c>
+      <c r="H122">
+        <v>10763</v>
+      </c>
+      <c r="I122">
+        <v>10763</v>
+      </c>
+      <c r="J122" t="s">
+        <v>4</v>
+      </c>
+      <c r="M122" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>24</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B123" t="s">
         <v>25</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C123" t="s">
         <v>26</v>
       </c>
-      <c r="D110" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110">
-        <v>2</v>
-      </c>
-      <c r="F110">
+      <c r="D123" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>2</v>
+      </c>
+      <c r="F123">
         <v>56</v>
       </c>
-      <c r="G110">
-        <v>10763</v>
-      </c>
-      <c r="H110">
-        <v>10763</v>
-      </c>
-      <c r="I110">
-        <v>10763</v>
-      </c>
-      <c r="J110" t="s">
-        <v>4</v>
-      </c>
-      <c r="M110" t="s">
+      <c r="G123">
+        <v>10763</v>
+      </c>
+      <c r="H123">
+        <v>10763</v>
+      </c>
+      <c r="I123">
+        <v>10763</v>
+      </c>
+      <c r="J123" t="s">
+        <v>4</v>
+      </c>
+      <c r="M123" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" t="s">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" t="s">
         <v>41</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C124" t="s">
         <v>3</v>
       </c>
-      <c r="D111" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111">
-        <v>4</v>
-      </c>
-      <c r="F111">
+      <c r="D124" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+      <c r="F124">
         <v>180</v>
       </c>
-      <c r="G111">
-        <v>10763</v>
-      </c>
-      <c r="H111">
-        <v>10763</v>
-      </c>
-      <c r="I111">
-        <v>10763</v>
-      </c>
-      <c r="J111" t="s">
-        <v>4</v>
-      </c>
-      <c r="M111" t="s">
+      <c r="G124">
+        <v>10763</v>
+      </c>
+      <c r="H124">
+        <v>10763</v>
+      </c>
+      <c r="I124">
+        <v>10763</v>
+      </c>
+      <c r="J124" t="s">
+        <v>4</v>
+      </c>
+      <c r="M124" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" t="s">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" t="s">
         <v>42</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C125" t="s">
         <v>1</v>
       </c>
-      <c r="D112" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112">
+      <c r="D125" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125">
         <v>31</v>
       </c>
-      <c r="F112">
+      <c r="F125">
         <v>4340</v>
       </c>
-      <c r="G112">
-        <v>10763</v>
-      </c>
-      <c r="H112">
-        <v>10763</v>
-      </c>
-      <c r="I112">
-        <v>10763</v>
-      </c>
-      <c r="J112" t="s">
-        <v>4</v>
-      </c>
-      <c r="M112" t="s">
+      <c r="G125">
+        <v>10763</v>
+      </c>
+      <c r="H125">
+        <v>10763</v>
+      </c>
+      <c r="I125">
+        <v>10763</v>
+      </c>
+      <c r="J125" t="s">
+        <v>4</v>
+      </c>
+      <c r="M125" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M112" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="CAP018_BKG_00001"/>
-        <filter val="CAP018_BKG_00003"/>
-        <filter val="CAP018_BKG_00007"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Loading test data from excel file
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Desktop\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asama\Github\Alaska-ITS\CG.iCargoTestAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A694A519-99FE-4BD4-9BB3-7B7BD84799BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E49357-D0FD-4FBD-9610-5B3FFA30964E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" activeTab="2" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
   <sheets>
     <sheet name="CAP018_BKG_00001" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="31">
   <si>
     <t>NONSCR</t>
   </si>
@@ -67,9 +67,6 @@
     <t>LAX</t>
   </si>
   <si>
-    <t>CAP018_BKG_00003</t>
-  </si>
-  <si>
     <t>CAP018_BKG_00001</t>
   </si>
   <si>
@@ -115,28 +112,28 @@
     <t>ANC</t>
   </si>
   <si>
+    <t>GOLDSTREAK</t>
+  </si>
+  <si>
+    <t>PET CONNECT</t>
+  </si>
+  <si>
+    <t>CAP018_BKG_00007</t>
+  </si>
+  <si>
+    <t>HNL</t>
+  </si>
+  <si>
+    <t>BOI</t>
+  </si>
+  <si>
+    <t>FAI</t>
+  </si>
+  <si>
+    <t>JFK</t>
+  </si>
+  <si>
     <t>SAN</t>
-  </si>
-  <si>
-    <t>JFK</t>
-  </si>
-  <si>
-    <t>GOLDSTREAK</t>
-  </si>
-  <si>
-    <t>PET CONNECT</t>
-  </si>
-  <si>
-    <t>CAP018_BKG_00007</t>
-  </si>
-  <si>
-    <t>HNL</t>
-  </si>
-  <si>
-    <t>BOI</t>
-  </si>
-  <si>
-    <t>FAI</t>
   </si>
 </sst>
 </file>
@@ -511,62 +508,62 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -596,10 +593,10 @@
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -631,18 +628,18 @@
         <v>4</v>
       </c>
       <c r="M3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -666,10 +663,10 @@
         <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -701,12 +698,12 @@
         <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -736,12 +733,12 @@
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -771,10 +768,10 @@
         <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -782,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -806,15 +803,15 @@
         <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -841,15 +838,15 @@
         <v>4</v>
       </c>
       <c r="M9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -876,18 +873,18 @@
         <v>4</v>
       </c>
       <c r="M10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -911,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="M11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -921,56 +918,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD5EE92-3539-4F36-A54E-54DD9A4C8224}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -998,16 +987,10 @@
       <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1033,22 +1016,16 @@
       <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1068,19 +1045,13 @@
       <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1102,12 +1073,6 @@
       </c>
       <c r="I5" t="s">
         <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1119,62 +1084,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BB6CDE-A36F-461E-AE8C-96C4C29B6083}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>9730</v>
@@ -1198,18 +1163,18 @@
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>9730</v>
@@ -1233,18 +1198,18 @@
         <v>4</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>9730</v>
@@ -1268,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in CAP018_BKG_00001 framework
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asama\Github\Alaska-ITS\CG.iCargoTestAutomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit_Anusha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E49357-D0FD-4FBD-9610-5B3FFA30964E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A699DABF-2671-4A52-AD0E-DBB581890BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
   <sheets>
     <sheet name="CAP018_BKG_00001" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>NONSCR</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>LAX</t>
-  </si>
-  <si>
-    <t>CAP018_BKG_00001</t>
   </si>
   <si>
     <t>Tags</t>
@@ -505,65 +502,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -589,14 +574,8 @@
       <c r="I2">
         <v>11377</v>
       </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -623,292 +602,6 @@
       </c>
       <c r="I3">
         <v>11377</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>11377</v>
-      </c>
-      <c r="H4">
-        <v>11377</v>
-      </c>
-      <c r="I4">
-        <v>11377</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2199</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>36</v>
-      </c>
-      <c r="G5">
-        <v>11377</v>
-      </c>
-      <c r="H5">
-        <v>11377</v>
-      </c>
-      <c r="I5">
-        <v>11377</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>11377</v>
-      </c>
-      <c r="H6">
-        <v>11377</v>
-      </c>
-      <c r="I6">
-        <v>11377</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>11377</v>
-      </c>
-      <c r="H7">
-        <v>11377</v>
-      </c>
-      <c r="I7">
-        <v>11377</v>
-      </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>36</v>
-      </c>
-      <c r="G8">
-        <v>11377</v>
-      </c>
-      <c r="H8">
-        <v>11377</v>
-      </c>
-      <c r="I8">
-        <v>11377</v>
-      </c>
-      <c r="J8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>11377</v>
-      </c>
-      <c r="H9">
-        <v>11377</v>
-      </c>
-      <c r="I9">
-        <v>11377</v>
-      </c>
-      <c r="J9" t="s">
-        <v>4</v>
-      </c>
-      <c r="M9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>11377</v>
-      </c>
-      <c r="H10">
-        <v>11377</v>
-      </c>
-      <c r="I10">
-        <v>11377</v>
-      </c>
-      <c r="J10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>36</v>
-      </c>
-      <c r="G11">
-        <v>11377</v>
-      </c>
-      <c r="H11">
-        <v>11377</v>
-      </c>
-      <c r="I11">
-        <v>11377</v>
-      </c>
-      <c r="J11" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -920,46 +613,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD5EE92-3539-4F36-A54E-54DD9A4C8224}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -988,9 +681,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1017,15 +710,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1046,12 +739,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1088,58 +781,58 @@
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>9730</v>
@@ -1163,18 +856,18 @@
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>9730</v>
@@ -1198,18 +891,18 @@
         <v>4</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>9730</v>
@@ -1233,7 +926,7 @@
         <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in some config
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -5,18 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Desktop\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit_Sprint 5\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B923E909-A5E7-4510-B590-0000BFDABC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E375925-0B06-43BF-9737-08C7BDCAE4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="7" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
   <sheets>
     <sheet name="CAP018_BKG_00001" sheetId="1" r:id="rId1"/>
     <sheet name="CAP018_BKG_00002" sheetId="4" r:id="rId2"/>
     <sheet name="CAP018_BKG_00003" sheetId="2" r:id="rId3"/>
-    <sheet name="CAP018_BKG_00007" sheetId="3" r:id="rId4"/>
+    <sheet name="CAP018_BKG_00004" sheetId="5" r:id="rId4"/>
+    <sheet name="CAP018_BKG_00005" sheetId="6" r:id="rId5"/>
+    <sheet name="CAP018_BKG_00007" sheetId="3" r:id="rId6"/>
+    <sheet name="CAP018_BKG_00008" sheetId="7" r:id="rId7"/>
+    <sheet name="CAP018_BKG_00009" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CAP018_BKG_00001!$A$1:$M$13</definedName>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="33">
   <si>
     <t>NONSCR</t>
   </si>
@@ -117,6 +121,30 @@
   </si>
   <si>
     <t>FAI</t>
+  </si>
+  <si>
+    <t>0316</t>
+  </si>
+  <si>
+    <t>JNU</t>
+  </si>
+  <si>
+    <t>PDX</t>
+  </si>
+  <si>
+    <t>BWI</t>
+  </si>
+  <si>
+    <t>0300</t>
+  </si>
+  <si>
+    <t>New AgentCode</t>
+  </si>
+  <si>
+    <t>MCO</t>
+  </si>
+  <si>
+    <t>DFW</t>
   </si>
 </sst>
 </file>
@@ -152,8 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -752,11 +782,195 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E58D6-2535-4DDC-92C3-2F70CE803C3D}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>10763</v>
+      </c>
+      <c r="H2">
+        <v>82165</v>
+      </c>
+      <c r="I2">
+        <v>82165</v>
+      </c>
+      <c r="J2">
+        <v>74428760</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68466B6-CC57-405A-AF55-279B16E6A348}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2199</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+      <c r="G2">
+        <v>10763</v>
+      </c>
+      <c r="H2">
+        <v>10763</v>
+      </c>
+      <c r="I2">
+        <v>10763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>950</v>
+      </c>
+      <c r="G3">
+        <v>10763</v>
+      </c>
+      <c r="H3">
+        <v>10763</v>
+      </c>
+      <c r="I3">
+        <v>10763</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BB6CDE-A36F-461E-AE8C-96C4C29B6083}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -880,4 +1094,272 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC666A12-8087-4101-828B-D04EDC9D9AAE}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>10763</v>
+      </c>
+      <c r="H2">
+        <v>10763</v>
+      </c>
+      <c r="I2">
+        <v>10763</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A363ED-10B1-4332-B456-5EADB439A750}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2199</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>360</v>
+      </c>
+      <c r="G2">
+        <v>10763</v>
+      </c>
+      <c r="H2">
+        <v>10763</v>
+      </c>
+      <c r="I2">
+        <v>10763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>775</v>
+      </c>
+      <c r="G3">
+        <v>10763</v>
+      </c>
+      <c r="H3">
+        <v>10763</v>
+      </c>
+      <c r="I3">
+        <v>10763</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>56</v>
+      </c>
+      <c r="G4">
+        <v>10763</v>
+      </c>
+      <c r="H4">
+        <v>10763</v>
+      </c>
+      <c r="I4">
+        <v>10763</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>180</v>
+      </c>
+      <c r="G5">
+        <v>10763</v>
+      </c>
+      <c r="H5">
+        <v>10763</v>
+      </c>
+      <c r="I5">
+        <v>10763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>4340</v>
+      </c>
+      <c r="G6">
+        <v>10763</v>
+      </c>
+      <c r="H6">
+        <v>10763</v>
+      </c>
+      <c r="I6">
+        <v>10763</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change in excel infra
</commit_message>
<xml_diff>
--- a/TestData/CAP018_MaintainBooking_TestData.xlsx
+++ b/TestData/CAP018_MaintainBooking_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit Sprint 7\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6789FB-973D-425A-B6A6-A6B9E296F9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B30438-D368-4F8D-8B1C-D2D6608834EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{957C75AA-B495-45B0-9A43-5BCB3C935300}"/>
   </bookViews>
   <sheets>
     <sheet name="CAP018_BKG_00001" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="34">
   <si>
     <t>NONSCR</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>DFW</t>
+  </si>
+  <si>
+    <t>SFO</t>
   </si>
 </sst>
 </file>
@@ -520,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9D18FD-7ADF-4352-8060-41965A331187}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,7 +567,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -596,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -622,7 +625,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -654,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -680,7 +683,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -709,7 +712,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -741,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -770,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -799,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -828,7 +831,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -857,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -886,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -915,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -944,7 +947,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -973,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -999,7 +1002,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -1028,7 +1031,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -1089,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -1115,7 +1118,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -1144,7 +1147,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -1176,7 +1179,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -1205,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -1234,7 +1237,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1263,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
@@ -1292,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1318,7 +1321,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -1350,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -1376,7 +1379,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
@@ -1405,7 +1408,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
@@ -1437,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -1466,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -1495,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -1524,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
@@ -1553,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -1579,7 +1582,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -1611,7 +1614,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -1637,7 +1640,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -1666,7 +1669,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
@@ -1698,7 +1701,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
@@ -1727,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -1756,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -1782,7 +1785,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
         <v>2</v>
@@ -1814,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
         <v>20</v>
@@ -1843,7 +1846,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
         <v>3</v>
@@ -1872,7 +1875,7 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -1901,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
         <v>20</v>
@@ -1930,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -1959,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
@@ -1988,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -2017,7 +2020,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -2043,7 +2046,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B53" t="s">
         <v>2</v>
@@ -2075,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -2101,7 +2104,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B55" t="s">
         <v>2</v>
@@ -2130,7 +2133,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
         <v>2</v>
@@ -2162,7 +2165,7 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
         <v>20</v>
@@ -2191,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
@@ -2220,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -2249,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>

</xml_diff>